<commit_message>
update:state cylinders and generate pdf
</commit_message>
<xml_diff>
--- a/api/output/infoExcel.xlsx
+++ b/api/output/infoExcel.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -431,81 +431,35 @@
         <v>Días</v>
       </c>
       <c r="G1" t="str">
-        <v>¿De Ñubles?</v>
+        <v>¿De Ñuble?</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>P10097001</v>
+        <v>test</v>
       </c>
       <c r="B2" t="str">
-        <v>Argón /Mix20</v>
+        <v>Nitrógeno Gaseoso</v>
       </c>
       <c r="C2" t="str">
         <v>10m3</v>
       </c>
       <c r="D2" t="str">
-        <v>2023-09-12</v>
+        <v>2023-11-15</v>
       </c>
       <c r="E2" t="str">
-        <v>2023-09-15</v>
+        <v>2023-11-15</v>
       </c>
       <c r="F2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G2" t="str">
-        <v>Si</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>P10097002</v>
-      </c>
-      <c r="B3" t="str">
-        <v>Argón /Mix20</v>
-      </c>
-      <c r="C3" t="str">
-        <v>10m3</v>
-      </c>
-      <c r="D3" t="str">
-        <v>2023-09-12</v>
-      </c>
-      <c r="E3" t="str">
-        <v>2023-09-13</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3" t="str">
-        <v>Si</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>P10097001</v>
-      </c>
-      <c r="B4" t="str">
-        <v>Argón /Mix20</v>
-      </c>
-      <c r="C4" t="str">
-        <v>10m3</v>
-      </c>
-      <c r="D4" t="str">
-        <v>2023-09-27</v>
-      </c>
-      <c r="E4" t="str">
-        <v>2023-09-29</v>
-      </c>
-      <c r="F4">
-        <v>2</v>
-      </c>
-      <c r="G4" t="str">
         <v>Si</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>